<commit_message>
Add dimensions on project images
</commit_message>
<xml_diff>
--- a/2_Prototype.xlsx
+++ b/2_Prototype.xlsx
@@ -707,6 +707,18 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -879,11 +891,27 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -895,67 +923,39 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,26 +1330,26 @@
     <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="1"/>
-    <col min="20" max="20" width="12.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" style="1" customWidth="1"/>
     <col min="22" max="22" width="40.42578125" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="14"/>
@@ -1366,12 +1366,12 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
     </row>
     <row r="3" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
@@ -1380,15 +1380,15 @@
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
     </row>
     <row r="4" spans="1:22" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1400,37 +1400,37 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
       <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="62"/>
-      <c r="J4" s="63"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
       <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="36" t="s">
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="68" t="s">
+      <c r="Q4" s="40"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="69"/>
+      <c r="T4" s="72"/>
       <c r="U4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1439,76 +1439,76 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="55"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="19"/>
       <c r="I5" s="16"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="64"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="67"/>
     </row>
     <row r="6" spans="1:22" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="56"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="24"/>
       <c r="I6" s="21"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="89"/>
-      <c r="S6" s="86"/>
-      <c r="T6" s="87"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="64"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="67"/>
     </row>
     <row r="7" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="57"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="60"/>
       <c r="H7" s="22"/>
       <c r="I7" s="17"/>
       <c r="J7" s="23"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="84"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="72"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="70"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="65"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="88"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="68"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>

</xml_diff>